<commit_message>
change people_widget to text area which makes more sense
</commit_message>
<xml_diff>
--- a/documentation/Example files/people_widget.xlsx
+++ b/documentation/Example files/people_widget.xlsx
@@ -106,9 +106,6 @@
     <t>WAGWAN?</t>
   </si>
   <si>
-    <t>select_or_add_multiple</t>
-  </si>
-  <si>
     <t>people</t>
   </si>
   <si>
@@ -118,10 +115,14 @@
     <t>Enter your friend's name!</t>
   </si>
   <si>
-    <t>"Ruben, Jessica"</t>
-  </si>
-  <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>textarea</t>
+  </si>
+  <si>
+    <t>"Ruben
+Jessica"</t>
   </si>
 </sst>
 </file>
@@ -582,7 +583,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -654,23 +655,23 @@
     </row>
     <row r="3" spans="1:13" ht="30">
       <c r="B3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:13">

</xml_diff>